<commit_message>
modified code to change one of analyses
</commit_message>
<xml_diff>
--- a/data/old-spreadsheets/21 03 03 AgNPs fish excretion models simulations.xlsx
+++ b/data/old-spreadsheets/21 03 03 AgNPs fish excretion models simulations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklem\Documents\Etudes\Trent\Xenopoulos lab\Projects\AgNP ELA lakes &amp; fish excretion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/AgNP-ELA_fish-excretion/data/old-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF1EF14-AE67-4E1A-947F-060159D81D7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF1EF14-AE67-4E1A-947F-060159D81D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8860" yWindow="4520" windowWidth="9600" windowHeight="4910" xr2:uid="{097E9588-E6E8-4050-963F-81EF450CE2DB}"/>
+    <workbookView minimized="1" xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="7270" xr2:uid="{097E9588-E6E8-4050-963F-81EF450CE2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fish excretion" sheetId="1" r:id="rId1"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98364C61-89D6-4CA9-B9CD-6190EAD1FA66}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>